<commit_message>
bug fixes and multiple files basic functionality
</commit_message>
<xml_diff>
--- a/api/components/toyige.xlsx
+++ b/api/components/toyige.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sepetab/Desktop/BINF6112_PROJECT/api/components/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sepetab/Desktop/MyOwnProjects/BINF6112_PROJECT/api/components/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3FC426E-7B0E-434F-AABC-CFFCEE10633A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FE1632B-EA1B-FF42-BCA1-82415F3E6D4E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2000" yWindow="7720" windowWidth="27440" windowHeight="13880" xr2:uid="{E6DAF190-D182-4CC3-B683-A8361AF653DC}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="26">
   <si>
     <t>#Date:Fri Sep 11 2020 12:33:12</t>
   </si>
@@ -106,6 +106,9 @@
   </si>
   <si>
     <t>Error</t>
+  </si>
+  <si>
+    <t>SNR</t>
   </si>
 </sst>
 </file>
@@ -474,12 +477,13 @@
   <dimension ref="A1:P9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P5" sqref="P5:P8"/>
+      <selection activeCell="P9" sqref="P9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="5" max="5" width="21.83203125" customWidth="1"/>
+    <col min="15" max="15" width="23.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.2">
@@ -608,7 +612,9 @@
       <c r="O5" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="P5" s="1"/>
+      <c r="P5" s="1" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
@@ -652,7 +658,9 @@
       <c r="O6" s="1">
         <v>2</v>
       </c>
-      <c r="P6" s="1"/>
+      <c r="P6" s="1">
+        <v>5</v>
+      </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
@@ -698,7 +706,9 @@
       <c r="O7" s="1">
         <v>4</v>
       </c>
-      <c r="P7" s="1"/>
+      <c r="P7" s="1">
+        <v>11</v>
+      </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
@@ -744,7 +754,9 @@
       <c r="O8" s="1">
         <v>4</v>
       </c>
-      <c r="P8" s="1"/>
+      <c r="P8" s="1">
+        <v>11</v>
+      </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A9" s="1"/>

</xml_diff>

<commit_message>
Initial Averaging for Clinical Epitope Ranking done
</commit_message>
<xml_diff>
--- a/api/components/toyige.xlsx
+++ b/api/components/toyige.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sepetab/Desktop/MyOwnProjects/BINF6112_PROJECT/api/components/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FE1632B-EA1B-FF42-BCA1-82415F3E6D4E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3BCF95E-A0E8-9349-B44E-DF578360BDF3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2000" yWindow="7720" windowWidth="27440" windowHeight="13880" xr2:uid="{E6DAF190-D182-4CC3-B683-A8361AF653DC}"/>
+    <workbookView xWindow="4540" yWindow="660" windowWidth="27440" windowHeight="13880" xr2:uid="{E6DAF190-D182-4CC3-B683-A8361AF653DC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="25">
   <si>
     <t>#Date:Fri Sep 11 2020 12:33:12</t>
   </si>
@@ -103,9 +103,6 @@
   </si>
   <si>
     <t>Arah1_overlapping 2</t>
-  </si>
-  <si>
-    <t>Error</t>
   </si>
   <si>
     <t>SNR</t>
@@ -476,8 +473,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B138514E-7367-46B9-B84F-74AF539EB20E}">
   <dimension ref="A1:P9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P9" sqref="P9"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="V10" sqref="V10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -613,7 +610,7 @@
         <v>18</v>
       </c>
       <c r="P5" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.2">
@@ -633,33 +630,37 @@
         <v>21</v>
       </c>
       <c r="F6" s="1">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="G6" s="1">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="H6" s="1">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="I6" s="1">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="J6" s="1">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="K6" s="1">
-        <v>2</v>
-      </c>
-      <c r="L6" s="1"/>
-      <c r="M6" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="L6" s="1">
+        <v>7</v>
+      </c>
+      <c r="M6" s="1">
+        <v>7</v>
+      </c>
       <c r="N6" s="1">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="O6" s="1">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="P6" s="1">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.2">
@@ -679,35 +680,37 @@
         <v>23</v>
       </c>
       <c r="F7" s="1">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="G7" s="1">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="H7" s="1">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="I7" s="1">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="J7" s="1">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="K7" s="1">
-        <v>4</v>
-      </c>
-      <c r="L7" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="M7" s="1"/>
+        <v>20</v>
+      </c>
+      <c r="L7" s="1">
+        <v>20</v>
+      </c>
+      <c r="M7" s="1">
+        <v>20</v>
+      </c>
       <c r="N7" s="1">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="O7" s="1">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="P7" s="1">
-        <v>11</v>
+        <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.2">
@@ -727,35 +730,37 @@
         <v>23</v>
       </c>
       <c r="F8" s="1">
-        <v>4</v>
+        <v>30</v>
       </c>
       <c r="G8" s="1">
-        <v>4</v>
+        <v>30</v>
       </c>
       <c r="H8" s="1">
-        <v>4</v>
+        <v>30</v>
       </c>
       <c r="I8" s="1">
-        <v>4</v>
+        <v>30</v>
       </c>
       <c r="J8" s="1">
-        <v>4</v>
+        <v>30</v>
       </c>
       <c r="K8" s="1">
-        <v>4</v>
-      </c>
-      <c r="L8" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="M8" s="1"/>
+        <v>30</v>
+      </c>
+      <c r="L8" s="1">
+        <v>30</v>
+      </c>
+      <c r="M8" s="1">
+        <v>30</v>
+      </c>
       <c r="N8" s="1">
-        <v>4</v>
+        <v>30</v>
       </c>
       <c r="O8" s="1">
-        <v>4</v>
+        <v>30</v>
       </c>
       <c r="P8" s="1">
-        <v>11</v>
+        <v>30</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.2">

</xml_diff>